<commit_message>
Update english evaluation grids for Word & PPT
</commit_message>
<xml_diff>
--- a/others_EN/inputs/html/AXS_assess_grid_PPT_EN.xlsx
+++ b/others_EN/inputs/html/AXS_assess_grid_PPT_EN.xlsx
@@ -19,58 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
-  <si>
-    <t>La langue du document est définie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La couleur n'est pas le seul moyen de véhiculer de l’information  </t>
-  </si>
-  <si>
-    <t>Les intitulés de liens sont explicites</t>
-  </si>
-  <si>
-    <t>Un masque est utilisé pour la mise en forme du document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les champs "Titre", "Auteur" et "Mots clefs" sont renseignés </t>
-  </si>
-  <si>
-    <t xml:space="preserve">En cas de changement de langue ponctuel (citations, …) : le changement est signalé </t>
-  </si>
-  <si>
-    <t>Il y a autant de masques de diapositives que de types de présentations nécessaires</t>
-  </si>
-  <si>
-    <t>Chaque diapositive a un titre qui lui est unique, concis et détectable par les lecteurs d'écrans JAWS et NVDA</t>
-  </si>
-  <si>
-    <t>L’accentuation sur les majuscules (ÀÉÈÊÏÔÙÇ) est conservée</t>
-  </si>
-  <si>
-    <t>Les acronymes ou expressions particulières sont évités ou explicités à la première occurrence</t>
-  </si>
-  <si>
-    <t>Police de caractères sans serif (Arial, Helvetica…) en corps 12 pixels minimum</t>
-  </si>
-  <si>
-    <t>Pas de phrases entièrement en majuscules et présence de majuscule en début de phrase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le texte est aligné à gauche (pas justifié) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">On utilise les attributs "Retrait et Espacement" (dans Clic droit &gt; Paragraphe) pour espacer le corps de texte (pas de retours chariots ou de tabulation) </t>
-  </si>
-  <si>
-    <t>Le contraste entre la couleur du contenu et celle du fond respecte : 
-o 4.5/1 pour du texte de taille standard (12 ou 16)
-o 3/1 pour texte de grande taille (150% ou 120% si gras de taille standard) 
-(Tester les contrastes avec Colour Contrast Analyser)</t>
-  </si>
-  <si>
-    <t>Les liens vers des fichiers téléchargeables indiquent le nom, le format, le poids et la langue du fichier (si celle-ci est différente de la langue principale du document en cours)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Créer des documents bureautiques accessibles</t>
   </si>
@@ -82,11 +31,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.access-for-all.ch/en/pdf-lab/pdf-accessibility-checker-pac.html </t>
-  </si>
-  <si>
-    <t>Les liens qui déclenchent l’ouverture d’une nouvelle fenêtre incluent la mention
- « nouvelle fenêtre » dans leur libellé (modifier le lien &gt; "Info-bulle")
-Exemple : "Anoo (nouvelle fenêtre)"</t>
   </si>
   <si>
     <t xml:space="preserve">paste here the result of the Office automated audit </t>
@@ -209,6 +153,55 @@
   </si>
   <si>
     <t>the appropriate and native functions are used in order to create lists</t>
+  </si>
+  <si>
+    <t>For every downloadable file, it is necessary to specify its name, type, size and language (if different of the presentation language)</t>
+  </si>
+  <si>
+    <t>Hyperlinks titles are simples and concises</t>
+  </si>
+  <si>
+    <t>The presentation of text should have a contrast ratio of at least 4.5:1
+you can download the Colour Contrast Analyser tool</t>
+  </si>
+  <si>
+    <t>Ensure that color is not the only means of conveying information</t>
+  </si>
+  <si>
+    <t>Use familiar sans serif fonts (such as Arial or Calibri), in a larger font size (18pt or larger).</t>
+  </si>
+  <si>
+    <t>Begin all sentences by a capital letter but avoid using all capital letters and excessive italics or underlines</t>
+  </si>
+  <si>
+    <t>Avoid justifying the text; prefer left alignment.</t>
+  </si>
+  <si>
+    <t>In order to add white space between sentences and paragraphs, use option: right click on the text and select Paragraph… &gt; Indents and Spacing</t>
+  </si>
+  <si>
+    <t>If necessary, keep accentuation on capital letters (example: É or Ç): use the Insert tab &gt; Symbol</t>
+  </si>
+  <si>
+    <t>Avoid abbreviations and acronyms; explain them at the first occurrence</t>
+  </si>
+  <si>
+    <t>Give every slide a unique and descriptive title</t>
+  </si>
+  <si>
+    <t>Title, author and tags fields have to be completed in tab File &gt; Info &gt; Properties.</t>
+  </si>
+  <si>
+    <t>The main language must be defined in the tab File &gt; Options &gt; Language</t>
+  </si>
+  <si>
+    <t>Every punctual change of language must be identified by selecting the text and: tab Review &gt; Language &gt; Set proofing language</t>
+  </si>
+  <si>
+    <t>Use the Slide Master view: select the View tab &gt; Slide Master to create or modify slides layouts</t>
+  </si>
+  <si>
+    <t>Create slide layouts for every type of slide</t>
   </si>
 </sst>
 </file>
@@ -828,10 +821,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:C24"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -844,341 +837,335 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B2" s="27"/>
       <c r="C2" s="28"/>
     </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" s="6" customFormat="1" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B5" s="27"/>
       <c r="C5" s="28"/>
     </row>
     <row r="6" spans="1:3" s="6" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" s="6" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:3" s="6" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="6" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="25"/>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="25"/>
     </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="25"/>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:4" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:4" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="25"/>
     </row>
-    <row r="20" spans="1:4" s="2" customFormat="1" ht="78.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B20" s="12"/>
       <c r="D20" s="22" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
     </row>
     <row r="22" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="25"/>
     </row>
     <row r="23" spans="1:4" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B24" s="24"/>
       <c r="C24" s="25"/>
     </row>
     <row r="25" spans="1:4" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
     </row>
     <row r="26" spans="1:4" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:4" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
     </row>
     <row r="28" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="25"/>
     </row>
     <row r="29" spans="1:4" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
     </row>
-    <row r="30" spans="1:4" s="2" customFormat="1" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
     </row>
-    <row r="31" spans="1:4" s="2" customFormat="1" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-    </row>
-    <row r="32" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-    </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="1:4" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+    </row>
+    <row r="33" spans="1:3" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-    </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="25"/>
-    </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
+    </row>
+    <row r="36" spans="1:3" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+    </row>
+    <row r="37" spans="1:3" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
     </row>
-    <row r="40" spans="1:3" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-    </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="24"/>
-      <c r="C41" s="25"/>
-    </row>
-    <row r="42" spans="1:3" s="14" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="24"/>
+      <c r="C40" s="25"/>
+    </row>
+    <row r="41" spans="1:3" s="14" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+    </row>
+    <row r="42" spans="1:3" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
     </row>
-    <row r="43" spans="1:3" s="2" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-    </row>
-    <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="25"/>
-    </row>
-    <row r="45" spans="1:3" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="24"/>
+      <c r="C43" s="25"/>
+    </row>
+    <row r="44" spans="1:3" s="2" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+    </row>
+    <row r="45" spans="1:3" s="4" customFormat="1" ht="31.5" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
     </row>
-    <row r="46" spans="1:3" s="4" customFormat="1" ht="31.5" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" s="4" customFormat="1" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
     </row>
-    <row r="47" spans="1:3" s="4" customFormat="1" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-    </row>
+    <row r="47" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="50" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="51" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="52" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1191,20 +1178,19 @@
     <row r="59" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="60" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="61" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A43:C43"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A40:C40"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A9:C9"/>
@@ -1232,12 +1218,12 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1257,7 +1243,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1265,13 +1251,13 @@
     </row>
     <row r="3" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
       <c r="B4" s="18" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1279,12 +1265,12 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1292,27 +1278,27 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>